<commit_message>
Ajout des premières versions des wireframe
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\Projet Symfony\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\Projet Symfony\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -206,12 +206,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -222,8 +219,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,7 +508,7 @@
   <dimension ref="A9:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,16 +520,16 @@
   <sheetData>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -540,7 +540,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
@@ -549,7 +549,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -558,7 +558,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -567,7 +567,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -576,7 +576,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
@@ -585,7 +585,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -596,7 +596,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
@@ -605,7 +605,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
@@ -614,7 +614,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
@@ -623,7 +623,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
@@ -643,7 +643,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
@@ -652,7 +652,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="3" t="s">

</xml_diff>